<commit_message>
Updated Work Breakdown Structure and Sprint Backlog xls
</commit_message>
<xml_diff>
--- a/Project/Phase_1/Sprint_1/Sprint Backlog.xlsx
+++ b/Project/Phase_1/Sprint_1/Sprint Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\JabRef\jabref\Project\Phase_1\Sprint_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E5C36B-333E-4357-BABE-117148D722A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E14EC2-37F4-4F30-A933-005F993E46BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6570" yWindow="6570" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4875" yWindow="2865" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint Backlog" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="72">
   <si>
     <t>Low - not required for now</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>OWNER</t>
-  </si>
-  <si>
     <t>DONE</t>
   </si>
   <si>
@@ -75,17 +72,188 @@
     <t xml:space="preserve">IN PROGRESS </t>
   </si>
   <si>
-    <t>USER STORIES (US)</t>
+    <t>Phase</t>
   </si>
   <si>
-    <t>Phase</t>
+    <t>Analyse Jabref codebase</t>
+  </si>
+  <si>
+    <t>Create github repository via forking</t>
+  </si>
+  <si>
+    <t>Elaborate the use-case description docx</t>
+  </si>
+  <si>
+    <t>Elaborate the code-smell report documents</t>
+  </si>
+  <si>
+    <t>Manage remote repository</t>
+  </si>
+  <si>
+    <t>Attend Planned Team meeting</t>
+  </si>
+  <si>
+    <t>Elaborate the design pattern report documents</t>
+  </si>
+  <si>
+    <t>Author of the task</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>Pedro Simoes 58674</t>
+  </si>
+  <si>
+    <t>Elaborate the general use-case diagram</t>
+  </si>
+  <si>
+    <t>Elaborate the Database Organization UC diagram</t>
+  </si>
+  <si>
+    <t>Bruno Ramos 52886</t>
+  </si>
+  <si>
+    <t>Elaborate the File Sharing UC diagram</t>
+  </si>
+  <si>
+    <t>Francisco Freire 58667</t>
+  </si>
+  <si>
+    <t>Francisco Pires 58208</t>
+  </si>
+  <si>
+    <t>Goncalo Vicencio 57944</t>
+  </si>
+  <si>
+    <t>Elaborate the Entry Collection UC diagram</t>
+  </si>
+  <si>
+    <t>Elaborate the Configurations Organization UC diagram</t>
+  </si>
+  <si>
+    <t>Elaborate the Cite(Citation) UC diagram</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Peer Review Database Organization UC diagram</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Peer Review Entry Collection UC diagram</t>
+  </si>
+  <si>
+    <t>Peer Review File Sharing UC diagram</t>
+  </si>
+  <si>
+    <t>Peer Review Configurations Organization UC diagram</t>
+  </si>
+  <si>
+    <t>Peer Review Cite(Citation) UC diagram</t>
+  </si>
+  <si>
+    <t>All members (during meeting)</t>
+  </si>
+  <si>
+    <t>Respective author of each diagram</t>
+  </si>
+  <si>
+    <t>Each member is free to search anywhere in the codebase, keeping communication up, so that it doesn't overlap with others.</t>
+  </si>
+  <si>
+    <t>Peer review Pedro's code-smell report documents</t>
+  </si>
+  <si>
+    <t>Peer review Bruno's code-smell report documents</t>
+  </si>
+  <si>
+    <t>Peer review Francisco Freire's code-smell report documents</t>
+  </si>
+  <si>
+    <t>Peer review Francisco Pires code-smell report documents</t>
+  </si>
+  <si>
+    <t>Peer review Goncalo's code-smell report documents</t>
+  </si>
+  <si>
+    <t>Francisco Freire 58667, Francisco Pires 58208, Goncalo Vicencio 57944</t>
+  </si>
+  <si>
+    <t>Francisco Pires 58208, Goncalo Vicencio 57944, Pedro Simoes 58674</t>
+  </si>
+  <si>
+    <t>Francisco Freire 58667, Bruno Ramos 52886, Pedro Simoes 58674</t>
+  </si>
+  <si>
+    <t>Francisco Freire 58667, Bruno Ramos 52886, Francisco Pires 58208</t>
+  </si>
+  <si>
+    <t>Scrum Master Assignment</t>
+  </si>
+  <si>
+    <t>Scrum Master Tasks</t>
+  </si>
+  <si>
+    <t>Peer review Pedro's design pattern report documents</t>
+  </si>
+  <si>
+    <t>Peer review Bruno's design pattern report documents</t>
+  </si>
+  <si>
+    <t>Peer review Francisco Freire's design pattern report documents</t>
+  </si>
+  <si>
+    <t>Peer review Francisco Pires design pattern report documents</t>
+  </si>
+  <si>
+    <t>All members</t>
+  </si>
+  <si>
+    <t>Analyse Jabref codebase to find design patterns</t>
+  </si>
+  <si>
+    <t>Analyse Jabref codebase to find code smells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structured Metrics Analysis </t>
+  </si>
+  <si>
+    <t>Chidamber-Kemerer Metrics report elaboration</t>
+  </si>
+  <si>
+    <t>Martin Packaging Metrics report elaboration</t>
+  </si>
+  <si>
+    <t>Complexity Metrics report elaboration</t>
+  </si>
+  <si>
+    <t>Lines of Code Metrics report elaboration</t>
+  </si>
+  <si>
+    <t>Bruno Ramos 52886, Francisco Pires 58208, Francisco Freire 28667</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All members </t>
+  </si>
+  <si>
+    <t>MOOD Metrics report elaboration</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Goncalo Vicencio 57944, Pedro Simoes 58674, Bruno Ramos 52886</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -94,10 +262,6 @@
     <font>
       <b/>
       <sz val="14"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -153,13 +317,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -181,6 +338,24 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4" tint="0.39997558519241921"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -273,68 +448,100 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -654,10 +861,10 @@
     <tabColor rgb="FFFFFF00"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB1000"/>
+  <dimension ref="A1:AB999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -672,27 +879,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="13" t="s">
+      <c r="B1" s="37">
+        <v>44536</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="13" t="s">
+      <c r="D1" s="35">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="39"/>
+      <c r="F1" s="36">
+        <v>27</v>
+      </c>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="38"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="35">
+        <v>1</v>
+      </c>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
@@ -702,57 +917,55 @@
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="36" t="s">
+      <c r="B4" s="10"/>
+      <c r="C4" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="35" t="s">
+      <c r="E4" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="F4" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="34" t="s">
+      <c r="G4" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="10"/>
-      <c r="AA4" s="10"/>
-      <c r="AB4" s="10"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="9"/>
+      <c r="AB4" s="9"/>
     </row>
     <row r="5" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -776,542 +989,805 @@
       <c r="AB5" s="4"/>
     </row>
     <row r="6" spans="1:28" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="28"/>
-      <c r="I6" s="27" t="s">
+      <c r="A6" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="30"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="24" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="28"/>
-      <c r="I7" s="7" t="s">
+      <c r="A7" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="30"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="I7" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="28"/>
-      <c r="I8" s="9" t="s">
+      <c r="A8" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="27"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="I8" s="8" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:28" ht="18" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="28"/>
-      <c r="I9" s="6" t="s">
+      <c r="A9" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="27"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:28" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="I10" s="8" t="s">
+      <c r="A10" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="27"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="I10" s="7" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="28"/>
-    </row>
-    <row r="12" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
-      <c r="U12" s="4"/>
-      <c r="V12" s="4"/>
-      <c r="W12" s="4"/>
-      <c r="X12" s="4"/>
-      <c r="Y12" s="4"/>
-      <c r="Z12" s="4"/>
-      <c r="AA12" s="4"/>
-      <c r="AB12" s="4"/>
-    </row>
-    <row r="13" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C13" s="43"/>
-      <c r="D13" s="26"/>
+      <c r="A11" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="27"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>32</v>
+      </c>
       <c r="E13" s="26"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-    </row>
-    <row r="14" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C14" s="44"/>
-      <c r="D14" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>35</v>
+      </c>
       <c r="E14" s="26"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-    </row>
-    <row r="15" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C15" s="44"/>
-      <c r="D15" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>37</v>
+      </c>
       <c r="E15" s="26"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-    </row>
-    <row r="16" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C16" s="44"/>
-      <c r="D16" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>38</v>
+      </c>
       <c r="E16" s="26"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-    </row>
-    <row r="17" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C17" s="44"/>
-      <c r="D17" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A17" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>39</v>
+      </c>
       <c r="E17" s="26"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-    </row>
-    <row r="18" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C18" s="44"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-    </row>
-    <row r="19" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C19" s="44"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-    </row>
-    <row r="20" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
-      <c r="W20" s="4"/>
-      <c r="X20" s="4"/>
-      <c r="Y20" s="4"/>
-      <c r="Z20" s="4"/>
-      <c r="AA20" s="4"/>
-      <c r="AB20" s="4"/>
-    </row>
-    <row r="21" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C21" s="45"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-    </row>
-    <row r="22" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C22" s="46"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-    </row>
-    <row r="23" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C23" s="46"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-    </row>
-    <row r="24" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C24" s="46"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-    </row>
-    <row r="25" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C25" s="46"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-    </row>
-    <row r="26" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C26" s="46"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-    </row>
-    <row r="27" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C27" s="46"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-    </row>
-    <row r="28" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
-      <c r="T28" s="4"/>
-      <c r="U28" s="4"/>
-      <c r="V28" s="4"/>
-      <c r="W28" s="4"/>
-      <c r="X28" s="4"/>
-      <c r="Y28" s="4"/>
-      <c r="Z28" s="4"/>
-      <c r="AA28" s="4"/>
-      <c r="AB28" s="4"/>
-    </row>
-    <row r="29" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C29" s="47"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-    </row>
-    <row r="30" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C30" s="42"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-    </row>
-    <row r="31" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C31" s="42"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-    </row>
-    <row r="32" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C32" s="42"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-    </row>
-    <row r="33" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C33" s="42"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-    </row>
-    <row r="34" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C34" s="42"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-    </row>
-    <row r="35" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C35" s="42"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-    </row>
-    <row r="36" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C36" s="42"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
-    </row>
-    <row r="37" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
-      <c r="O37" s="4"/>
-      <c r="P37" s="4"/>
-      <c r="Q37" s="4"/>
-      <c r="R37" s="4"/>
-      <c r="S37" s="4"/>
-      <c r="T37" s="4"/>
-      <c r="U37" s="4"/>
-      <c r="V37" s="4"/>
-      <c r="W37" s="4"/>
-      <c r="X37" s="4"/>
-      <c r="Y37" s="4"/>
-      <c r="Z37" s="4"/>
-      <c r="AA37" s="4"/>
-      <c r="AB37" s="4"/>
-    </row>
-    <row r="38" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C38" s="20"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-    </row>
-    <row r="39" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C39" s="5"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-    </row>
-    <row r="40" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C40" s="5"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-    </row>
-    <row r="41" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C41" s="5"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-    </row>
-    <row r="42" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C42" s="5"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-    </row>
-    <row r="43" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C43" s="5"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-    </row>
-    <row r="44" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C44" s="5"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
-    </row>
-    <row r="45" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C45" s="5"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
-    </row>
-    <row r="46" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C46" s="5"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
-    </row>
-    <row r="47" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
-      <c r="P47" s="4"/>
-      <c r="Q47" s="4"/>
-      <c r="R47" s="4"/>
-      <c r="S47" s="4"/>
-      <c r="T47" s="4"/>
-      <c r="U47" s="4"/>
-      <c r="V47" s="4"/>
-      <c r="W47" s="4"/>
-      <c r="X47" s="4"/>
-      <c r="Y47" s="4"/>
-      <c r="Z47" s="4"/>
-      <c r="AA47" s="4"/>
-      <c r="AB47" s="4"/>
-    </row>
-    <row r="48" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C48" s="3"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-    </row>
-    <row r="49" spans="3:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C49" s="3"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="15"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-    </row>
-    <row r="50" spans="3:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C50" s="3"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-    </row>
-    <row r="51" spans="3:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C51" s="3"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-    </row>
-    <row r="52" spans="3:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C52" s="3"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-    </row>
-    <row r="53" spans="3:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C53" s="3"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-    </row>
-    <row r="54" spans="3:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C54" s="3"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-    </row>
-    <row r="55" spans="3:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F17" s="26"/>
+      <c r="G17" s="25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A18" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A19" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A20" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="38" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="22"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="56" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A23" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="22"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="56" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="22"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="56" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="22"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="56" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A26" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="22"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="56" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A27" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="56" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A28" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="56" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="38" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+    </row>
+    <row r="30" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A30" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="E30" s="20"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="57" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A31" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" s="20"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="57" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="38" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+    </row>
+    <row r="33" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A33" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="58" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A34" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="58" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A35" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="58" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A36" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" s="52" t="s">
+        <v>56</v>
+      </c>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="58" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A37" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="51" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="58" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A38" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="58" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A39" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="D39" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="58" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A40" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="58" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A41" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="58" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="38" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+    </row>
+    <row r="43" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A43" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="D43" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="E43" s="18"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A44" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="D44" s="53" t="s">
+        <v>63</v>
+      </c>
+      <c r="E44" s="18"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A45" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="D45" s="53" t="s">
+        <v>64</v>
+      </c>
+      <c r="E45" s="18"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A46" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="C46" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="E46" s="18"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A47" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A48" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="C48" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="D48" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A49" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C49" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="D49" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A50" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D50" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+    </row>
+    <row r="52" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+    </row>
+    <row r="53" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+    </row>
+    <row r="54" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+    </row>
+    <row r="55" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C55" s="3"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="15"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-    </row>
-    <row r="56" spans="3:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+    </row>
+    <row r="56" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C56" s="3"/>
-      <c r="D56" s="15"/>
-      <c r="E56" s="15"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-    </row>
-    <row r="57" spans="3:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C57" s="3"/>
-      <c r="D57" s="15"/>
-      <c r="E57" s="15"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-    </row>
-    <row r="58" spans="3:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+    </row>
+    <row r="57" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+    </row>
+    <row r="58" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="3:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="3:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
     </row>
-    <row r="61" spans="3:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="3:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
     </row>
-    <row r="63" spans="3:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
     </row>
-    <row r="64" spans="3:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="1"/>
@@ -6927,19 +7403,8 @@
       <c r="F999" s="1"/>
       <c r="G999" s="1"/>
     </row>
-    <row r="1000" spans="4:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D1000" s="2"/>
-      <c r="E1000" s="2"/>
-      <c r="F1000" s="1"/>
-      <c r="G1000" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="C6:C11"/>
-    <mergeCell ref="C13:C19"/>
-    <mergeCell ref="C21:C27"/>
-    <mergeCell ref="C29:C36"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified Scrum board and sprint backlog
</commit_message>
<xml_diff>
--- a/Project/Phase_1/Sprint_1/Sprint Backlog.xlsx
+++ b/Project/Phase_1/Sprint_1/Sprint Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\JabRef\jabref\Project\Phase_1\Sprint_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E14EC2-37F4-4F30-A933-005F993E46BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5702CBE2-BFE0-44F1-B9C8-DDB3AED97C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4875" yWindow="2865" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2670" yWindow="945" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint Backlog" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="73">
   <si>
     <t>Low - not required for now</t>
   </si>
@@ -248,6 +248,9 @@
   <si>
     <t>Goncalo Vicencio 57944, Pedro Simoes 58674, Bruno Ramos 52886</t>
   </si>
+  <si>
+    <t>Merging of all files in a final deliverable and reviewing</t>
+  </si>
 </sst>
 </file>
 
@@ -448,7 +451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -542,6 +545,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -863,8 +869,8 @@
   </sheetPr>
   <dimension ref="A1:AB999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1694,7 +1700,7 @@
       <c r="C50" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="D50" s="53" t="s">
+      <c r="D50" s="54" t="s">
         <v>19</v>
       </c>
       <c r="E50" s="18"/>
@@ -1703,12 +1709,21 @@
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
+    <row r="51" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A51" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C51" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="D51" s="60" t="s">
+        <v>72</v>
+      </c>
       <c r="E51" s="18"/>
       <c r="F51" s="18"/>
-      <c r="G51" s="18"/>
+      <c r="G51" s="59" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="52" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C52" s="18"/>

</xml_diff>